<commit_message>
updating work so far
</commit_message>
<xml_diff>
--- a/excel/genes.xlsx
+++ b/excel/genes.xlsx
@@ -14,9 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>genbank</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>annotated</t>
+  </si>
+  <si>
+    <t>seedOrtholog</t>
+  </si>
+  <si>
+    <t>evalueEggnog</t>
+  </si>
+  <si>
+    <t>scoreEggnog</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>preferredName</t>
+  </si>
+  <si>
+    <t>clusterId_id</t>
+  </si>
+  <si>
+    <t>QWERTY</t>
+  </si>
+  <si>
+    <t>ACGATGCTAGTATCG</t>
+  </si>
+  <si>
+    <t>Sed ut perspiciatis unde omnis iste natus error si</t>
+  </si>
+  <si>
+    <t>PAR3</t>
   </si>
 </sst>
 </file>
@@ -374,23 +413,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
+    <row r="1" spans="1:11">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>